<commit_message>
se empieza a modificar el menu inferior para hacerlo reutilizable en cada escenario.
</commit_message>
<xml_diff>
--- a/extra/Menu inferior.xlsx
+++ b/extra/Menu inferior.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62ED148E-0DBF-4683-84AB-F4F1F4318E7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332E767B-A7F8-47F2-A302-1B1A090798AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
   <si>
     <t>MENU INICIAL</t>
   </si>
@@ -35,13 +35,350 @@
   </si>
   <si>
     <t>City</t>
+  </si>
+  <si>
+    <t>Mover a</t>
+  </si>
+  <si>
+    <t>Tienda</t>
+  </si>
+  <si>
+    <t>Gremio</t>
+  </si>
+  <si>
+    <t>Portal</t>
+  </si>
+  <si>
+    <t>Posada</t>
+  </si>
+  <si>
+    <t>Confirmar</t>
+  </si>
+  <si>
+    <t>Cancelar</t>
+  </si>
+  <si>
+    <t>Personaje</t>
+  </si>
+  <si>
+    <t>Inventario</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Guardar</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> verificarPartida()</t>
+    </r>
+  </si>
+  <si>
+    <t>Comprar</t>
+  </si>
+  <si>
+    <t>Vender</t>
+  </si>
+  <si>
+    <t>Volver a ciudad</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> loadScenario() + cambio de ubicacion </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ShowBuyList()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ShowSellList()</t>
+    </r>
+  </si>
+  <si>
+    <t>Misiones</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ShowQuest()</t>
+    </r>
+  </si>
+  <si>
+    <t>Descansar</t>
+  </si>
+  <si>
+    <t>quieres una habitacion para descansar? Sale  ### G</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Cancelar  ( </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9C5700"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> loadScenario() + cambio de ubicacion )</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9C5700"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> loadScenario() + cambio de ubicacion </t>
+    </r>
+  </si>
+  <si>
+    <t>Explorar Area</t>
+  </si>
+  <si>
+    <t>(mostrar lista de areas para seleccionar)</t>
+  </si>
+  <si>
+    <t>Battle</t>
+  </si>
+  <si>
+    <t>Explorar</t>
+  </si>
+  <si>
+    <t>Area #</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ExplorarArea()</t>
+    </r>
+  </si>
+  <si>
+    <t>Atacar</t>
+  </si>
+  <si>
+    <t>Objeto</t>
+  </si>
+  <si>
+    <t>Huir</t>
+  </si>
+  <si>
+    <t>Habilidad</t>
+  </si>
+  <si>
+    <t>Deseas atacar a X?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ShowHability() + seleccionar habilidad</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ShowObjectBattle() + seleccionar object</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> EscapeFromBattle() + confirmar</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,8 +394,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -71,8 +430,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -80,20 +455,195 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -372,40 +922,484 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="70.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="35.77734375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="70.77734375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="30.77734375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="46" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="18" t="s">
         <v>4</v>
       </c>
+      <c r="B2" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="18"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="18"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="18"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="18"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="18"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="18"/>
+      <c r="B11" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="18"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="18"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="18"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="18"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="20"/>
+      <c r="B16" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="18"/>
+      <c r="B18" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="18"/>
+      <c r="B19" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="18"/>
+      <c r="B21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="18"/>
+      <c r="B24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="18"/>
+      <c r="B25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="18"/>
+      <c r="B28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="18"/>
+      <c r="B30" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="18"/>
+      <c r="B35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="18"/>
+      <c r="B36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="24"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="24"/>
+      <c r="B39" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="24"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="24"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="24"/>
+      <c r="B42" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="24"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="24"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="24"/>
+      <c r="B45" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="A37:A45"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B30:B34"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="A29:A36"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="A2:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A20:A21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>